<commit_message>
database displays on GUI
</commit_message>
<xml_diff>
--- a/movie_ratings.xlsx
+++ b/movie_ratings.xlsx
@@ -98,34 +98,34 @@
     <t>Who Is America?</t>
   </si>
   <si>
+    <t>A Star Is Born</t>
+  </si>
+  <si>
+    <t>136 min</t>
+  </si>
+  <si>
+    <t>Tom Clancy's Jack Ryan</t>
+  </si>
+  <si>
+    <t>60 min</t>
+  </si>
+  <si>
+    <t>Bodyguard</t>
+  </si>
+  <si>
+    <t>Killing Eve</t>
+  </si>
+  <si>
+    <t>43 min</t>
+  </si>
+  <si>
+    <t>Wild Wild Country</t>
+  </si>
+  <si>
+    <t>401 min</t>
+  </si>
+  <si>
     <t>A Discovery of Witches</t>
-  </si>
-  <si>
-    <t>60 min</t>
-  </si>
-  <si>
-    <t>A Star Is Born</t>
-  </si>
-  <si>
-    <t>136 min</t>
-  </si>
-  <si>
-    <t>Tom Clancy's Jack Ryan</t>
-  </si>
-  <si>
-    <t>Bodyguard</t>
-  </si>
-  <si>
-    <t>Killing Eve</t>
-  </si>
-  <si>
-    <t>43 min</t>
-  </si>
-  <si>
-    <t>Wild Wild Country</t>
-  </si>
-  <si>
-    <t>401 min</t>
   </si>
   <si>
     <t>Stree</t>
@@ -1777,7 +1777,7 @@
         <v>2018</v>
       </c>
       <c r="D16" t="n">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
@@ -1814,7 +1814,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1831,7 +1831,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1839,7 +1839,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" t="n">
         <v>2018</v>
@@ -1848,7 +1848,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1856,7 +1856,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" t="n">
         <v>2018</v>
@@ -1865,7 +1865,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1916,7 +1916,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1933,7 +1933,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1950,7 +1950,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2001,7 +2001,7 @@
         <v>8.1</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2137,7 +2137,7 @@
         <v>7.9</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2154,7 +2154,7 @@
         <v>7.9</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2188,7 +2188,7 @@
         <v>7.9</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2239,7 +2239,7 @@
         <v>7.8</v>
       </c>
       <c r="E43" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2324,7 +2324,7 @@
         <v>7.7</v>
       </c>
       <c r="E48" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2341,7 +2341,7 @@
         <v>7.7</v>
       </c>
       <c r="E49" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2358,7 +2358,7 @@
         <v>7.7</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2562,7 +2562,7 @@
         <v>8.6</v>
       </c>
       <c r="E62" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2596,7 +2596,7 @@
         <v>8.6</v>
       </c>
       <c r="E64" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2613,7 +2613,7 @@
         <v>8.6</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2630,7 +2630,7 @@
         <v>8.6</v>
       </c>
       <c r="E66" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2664,7 +2664,7 @@
         <v>8.5</v>
       </c>
       <c r="E68" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2698,7 +2698,7 @@
         <v>8.4</v>
       </c>
       <c r="E70" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2715,7 +2715,7 @@
         <v>8.4</v>
       </c>
       <c r="E71" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2732,7 +2732,7 @@
         <v>8.4</v>
       </c>
       <c r="E72" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2834,7 +2834,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E78" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2885,7 +2885,7 @@
         <v>8.1</v>
       </c>
       <c r="E81" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2902,7 +2902,7 @@
         <v>8.1</v>
       </c>
       <c r="E82" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3038,7 +3038,7 @@
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -3208,7 +3208,7 @@
         <v>7.7</v>
       </c>
       <c r="E100" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3378,7 +3378,7 @@
         <v>7.6</v>
       </c>
       <c r="E110" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -3514,7 +3514,7 @@
         <v>8.699999999999999</v>
       </c>
       <c r="E118" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3531,7 +3531,7 @@
         <v>8.6</v>
       </c>
       <c r="E119" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3616,7 +3616,7 @@
         <v>8.4</v>
       </c>
       <c r="E124" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3633,7 +3633,7 @@
         <v>8.4</v>
       </c>
       <c r="E125" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3650,7 +3650,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E126" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3684,7 +3684,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E128" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3786,7 +3786,7 @@
         <v>8.1</v>
       </c>
       <c r="E134" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -4092,7 +4092,7 @@
         <v>7.7</v>
       </c>
       <c r="E152" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -4109,7 +4109,7 @@
         <v>7.7</v>
       </c>
       <c r="E153" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -4296,7 +4296,7 @@
         <v>8.699999999999999</v>
       </c>
       <c r="E164" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -4364,7 +4364,7 @@
         <v>8.4</v>
       </c>
       <c r="E168" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -4381,7 +4381,7 @@
         <v>8.4</v>
       </c>
       <c r="E169" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -4432,7 +4432,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E172" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4568,7 +4568,7 @@
         <v>8.1</v>
       </c>
       <c r="E180" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4619,7 +4619,7 @@
         <v>8</v>
       </c>
       <c r="E183" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4721,7 +4721,7 @@
         <v>8</v>
       </c>
       <c r="E189" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5061,7 +5061,7 @@
         <v>7.6</v>
       </c>
       <c r="E209" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -5316,7 +5316,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E224" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -5333,7 +5333,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="E225" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -5384,7 +5384,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E228" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -5401,7 +5401,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="E229" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -5520,7 +5520,7 @@
         <v>8.1</v>
       </c>
       <c r="E236" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -5639,7 +5639,7 @@
         <v>8</v>
       </c>
       <c r="E243" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -5707,7 +5707,7 @@
         <v>7.9</v>
       </c>
       <c r="E247" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -5741,7 +5741,7 @@
         <v>7.8</v>
       </c>
       <c r="E249" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="250" spans="1:5">
@@ -5809,7 +5809,7 @@
         <v>7.8</v>
       </c>
       <c r="E253" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -5979,7 +5979,7 @@
         <v>7.6</v>
       </c>
       <c r="E263" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="264" spans="1:5">

</xml_diff>